<commit_message>
changed name to matchsync
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-nmdp-preferred-product-cs.xlsx
+++ b/docs/CodeSystem-nmdp-preferred-product-cs.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-12-01T09:35:21-06:00</t>
+    <t>2023-01-12T09:36:27-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>NMDP Preferred Product for MatchSource patient</t>
+    <t>NMDP Preferred Product for MatchSync patient</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>